<commit_message>
albert robustness test results
</commit_message>
<xml_diff>
--- a/experiments/evaluation/llm-based/albert-base-v2_15/original_remove/rem1/incorrect_predictions.xlsx
+++ b/experiments/evaluation/llm-based/albert-base-v2_15/original_remove/rem1/incorrect_predictions.xlsx
@@ -466,17 +466,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Current elevation above nnn Fly with caution .</t>
+          <t>Critically low power Aircraft is landing .</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Current elevation above nnn</t>
+          <t>Critically low power</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0-3</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -491,17 +491,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Current elevation above nnn Fly with caution .</t>
+          <t>Critically low power Aircraft is landing .</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Fly with caution</t>
+          <t>Aircraft is landing</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4-6</t>
+          <t>3-5</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -512,26 +512,26 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Critically Low Voltage Aircraft will land .</t>
+          <t>Critically low power Aircraft is landing .</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Critically Low Voltage</t>
+          <t>Critically low power Aircraft is landing</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>0-5</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -541,17 +541,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Critically Low Voltage Aircraft will land .</t>
+          <t>Backward Obstacle Sensing is not functioning Ambient Light is too weak .</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Aircraft will land</t>
+          <t>Backward Obstacle Sensing is not functioning</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3-5</t>
+          <t>0-5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -566,47 +566,47 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Critically Low Voltage Aircraft will land .</t>
+          <t>Backward Obstacle Sensing is not functioning Ambient Light is too weak .</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Critically Low Voltage Aircraft will land</t>
+          <t>Ambient Light is too weak</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0-5</t>
+          <t>6-10</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Missing</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Aircraft is close to the Home Point Initiating Return to Home will now trigger Auto Landing .</t>
+          <t>Backward Obstacle Sensing is not functioning Ambient Light is too weak .</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Aircraft is close to the Home Point</t>
+          <t>Backward Obstacle Sensing is not functioning Ambient Light is too weak</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0-6</t>
+          <t>0-10</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -616,17 +616,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Aircraft is close to the Home Point Initiating Return to Home will now trigger Auto Landing .</t>
+          <t>SD card speed low Change card .</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Initiating Return to Home will now trigger Auto Landing</t>
+          <t>SD card speed low</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>7-15</t>
+          <t>0-3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -637,21 +637,21 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Extra payload detected Max altitude set to nnn and max distance set to nnn to ensure flight safety .</t>
+          <t>SD card speed low Change card .</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Extra payload detected</t>
+          <t>Change card</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>4-5</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -662,26 +662,26 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Extra payload detected Max altitude set to nnn and max distance set to nnn to ensure flight safety .</t>
+          <t>SD card speed low Change card .</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Max altitude set to nnn and max distance set to nnn to ensure flight safety</t>
+          <t>SD card speed low Change card</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3-17</t>
+          <t>0-5</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -691,42 +691,42 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Extra payload detected Max altitude set to nnn and max distance set to nnn to ensure flight safety .</t>
+          <t>Low Power Returning home .</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Extra payload detected Max altitude set to nnn and max distance set to nnn to ensure flight safety</t>
+          <t>Low Power</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0-17</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Missing</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Aircraft ActiveTrack available at max speed When exceeding nnn, Obstacle Avoidance is not available .</t>
+          <t>Low Power Returning home .</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Aircraft ActiveTrack available at max speed</t>
+          <t>Returning home</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0-5</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -737,26 +737,26 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Aircraft ActiveTrack available at max speed When exceeding nnn, Obstacle Avoidance is not available .</t>
+          <t>Low Power Returning home .</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>When exceeding nnn, Obstacle Avoidance is not available</t>
+          <t>Low Power Returning home</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>6-13</t>
+          <t>0-3</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -766,42 +766,42 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Aircraft ActiveTrack available at max speed When exceeding nnn, Obstacle Avoidance is not available .</t>
+          <t>SD card full Change card or delete files .</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Obstacle Avoidance is not available</t>
+          <t>SD card full</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>9-13</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Missing</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Landing Protection Activated Aircraft will decelerate during landing .</t>
+          <t>SD card full Change card or delete files .</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Landing Protection Activated</t>
+          <t>Change card or delete files</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>3-7</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -812,26 +812,26 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Landing Protection Activated Aircraft will decelerate during landing .</t>
+          <t>SD card full Change card or delete files .</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Aircraft will decelerate during landing</t>
+          <t>SD card full Change card or delete files</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3-7</t>
+          <t>0-7</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -841,42 +841,42 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Landing Protection Activated Aircraft will decelerate during landing .</t>
+          <t>Precision Landing Rectifying aircraft position .</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Landing Protection Activated Aircraft will decelerate during landing</t>
+          <t>Precision Landing</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0-7</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Missing</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Forward vision sensor calibration error Auto calibration in progress .</t>
+          <t>Precision Landing Rectifying aircraft position .</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Forward vision sensor calibration error</t>
+          <t>Rectifying aircraft position</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0-4</t>
+          <t>2-4</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -887,26 +887,26 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Forward vision sensor calibration error Auto calibration in progress .</t>
+          <t>Precision Landing Rectifying aircraft position .</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Auto calibration in progress</t>
+          <t>Precision Landing Rectifying aircraft position</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5-8</t>
+          <t>0-4</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -916,42 +916,42 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Forward vision sensor calibration error Auto calibration in progress .</t>
+          <t>Aircraft ActiveTrack available at max speed When exceeding nnn, Obstacle Avoidance is not available .</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Forward vision sensor calibration error Auto calibration in progress</t>
+          <t>Aircraft ActiveTrack available at max speed</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0-8</t>
+          <t>0-5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Missing</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Forward Obstacle Sensing is not functioning Ambient Light is too weak .</t>
+          <t>Aircraft ActiveTrack available at max speed When exceeding nnn, Obstacle Avoidance is not available .</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Forward Obstacle Sensing is not functioning</t>
+          <t>When exceeding nnn, Obstacle Avoidance is not available</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0-5</t>
+          <t>6-13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -962,26 +962,26 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Forward Obstacle Sensing is not functioning Ambient Light is too weak .</t>
+          <t>Aircraft ActiveTrack available at max speed When exceeding nnn, Obstacle Avoidance is not available .</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Ambient Light is too weak</t>
+          <t>Obstacle Avoidance is not available</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>6-10</t>
+          <t>9-13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -991,42 +991,42 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Forward Obstacle Sensing is not functioning Ambient Light is too weak .</t>
+          <t>Mobile device CPU fully loaded Related performance will be affected .</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Forward Obstacle Sensing is not functioning Ambient Light is too weak</t>
+          <t>Mobile device CPU fully loaded</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0-10</t>
+          <t>0-4</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Missing</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SD card speed low Change card .</t>
+          <t>Mobile device CPU fully loaded Related performance will be affected .</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>SD card speed low</t>
+          <t>Related performance will be affected</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0-3</t>
+          <t>5-9</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1037,26 +1037,26 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SD card speed low Change card .</t>
+          <t>Mobile device CPU fully loaded Related performance will be affected .</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Change card</t>
+          <t>Mobile device CPU fully loaded Related performance will be affected</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>4-5</t>
+          <t>0-9</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -1066,12 +1066,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SD card speed low Change card .</t>
+          <t>Forward Obstacle Sensing is not functioning Ambient Light is too weak .</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>SD card speed low Change card</t>
+          <t>Forward Obstacle Sensing is not functioning</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1081,27 +1081,27 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Missing</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Compass Error Compass direction is not the same with IMU .</t>
+          <t>Forward Obstacle Sensing is not functioning Ambient Light is too weak .</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Compass Error</t>
+          <t>Ambient Light is too weak</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>6-10</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1112,26 +1112,26 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Compass Error Compass direction is not the same with IMU .</t>
+          <t>Forward Obstacle Sensing is not functioning Ambient Light is too weak .</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Compass direction is not the same with IMU</t>
+          <t>Forward Obstacle Sensing is not functioning Ambient Light is too weak</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2-9</t>
+          <t>0-10</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -1141,42 +1141,42 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Compass Error Compass direction is not the same with IMU .</t>
+          <t>Extra payload detected Max altitude set to nnn and max distance set to nnn to ensure flight safety .</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Compass Error Compass direction is not the same with IMU</t>
+          <t>Extra payload detected</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0-9</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Missing</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Backward Obstacle Sensing is not functioning Ambient Light is too weak .</t>
+          <t>Extra payload detected Max altitude set to nnn and max distance set to nnn to ensure flight safety .</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Backward Obstacle Sensing is not functioning</t>
+          <t>Max altitude set to nnn and max distance set to nnn to ensure flight safety</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0-5</t>
+          <t>3-17</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1187,26 +1187,26 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Backward Obstacle Sensing is not functioning Ambient Light is too weak .</t>
+          <t>Extra payload detected Max altitude set to nnn and max distance set to nnn to ensure flight safety .</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Ambient Light is too weak</t>
+          <t>Extra payload detected Max altitude set to nnn and max distance set to nnn to ensure flight safety</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>6-10</t>
+          <t>0-17</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -1216,42 +1216,42 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Backward Obstacle Sensing is not functioning Ambient Light is too weak .</t>
+          <t>Battery error Aircraft returning to home automatically .</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Backward Obstacle Sensing is not functioning Ambient Light is too weak</t>
+          <t>Battery error</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0-10</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Missing</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Mobile device CPU fully loaded Related performance will be affected .</t>
+          <t>Battery error Aircraft returning to home automatically .</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Mobile device CPU fully loaded</t>
+          <t>Aircraft returning to home automatically</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0-4</t>
+          <t>2-6</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1262,26 +1262,26 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Mobile device CPU fully loaded Related performance will be affected .</t>
+          <t>Battery error Aircraft returning to home automatically .</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Related performance will be affected</t>
+          <t>Battery error Aircraft returning to home automatically</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>5-9</t>
+          <t>0-6</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -1291,42 +1291,42 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Mobile device CPU fully loaded Related performance will be affected .</t>
+          <t>Precision Landing Locating Landing Point .</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Mobile device CPU fully loaded Related performance will be affected</t>
+          <t>Precision Landing</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0-9</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Missing</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Low Power Returning home .</t>
+          <t>Precision Landing Locating Landing Point .</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Low Power</t>
+          <t>Locating Landing Point</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>2-4</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1337,26 +1337,26 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Low Power Returning home .</t>
+          <t>Precision Landing Locating Landing Point .</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Returning home</t>
+          <t>Precision Landing Locating Landing Point</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2-3</t>
+          <t>0-4</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -1366,12 +1366,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Low Power Returning home .</t>
+          <t>Current elevation above nnn Fly with caution .</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Low Power Returning home</t>
+          <t>Current elevation above nnn</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1381,27 +1381,27 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Missing</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Propeller Guard Mounted Propeller Guard mounted Forward Obstacle Sensing will be automatically switched off .</t>
+          <t>Current elevation above nnn Fly with caution .</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Propeller Guard Mounted Propeller Guard mounted</t>
+          <t>Fly with caution</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0-5</t>
+          <t>4-6</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1416,17 +1416,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Propeller Guard Mounted Propeller Guard mounted Forward Obstacle Sensing will be automatically switched off .</t>
+          <t>Aircraft is close to the Home Point Initiating Return to Home will now trigger Auto Landing .</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Forward Obstacle Sensing will be automatically switched off</t>
+          <t>Aircraft is close to the Home Point</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>6-13</t>
+          <t>0-6</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1441,22 +1441,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Propeller Guard Mounted Propeller Guard mounted Forward Obstacle Sensing will be automatically switched off .</t>
+          <t>Aircraft is close to the Home Point Initiating Return to Home will now trigger Auto Landing .</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Propeller Guard Mounted Propeller Guard mounted Forward Obstacle Sensing will be automatically switched off</t>
+          <t>Initiating Return to Home will now trigger Auto Landing</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>0-13</t>
+          <t>7-15</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Missing</t>
         </is>
       </c>
     </row>
@@ -1466,17 +1466,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Aircraft processor overheated Automatically returning to home .</t>
+          <t>Forward vision sensor calibration error Auto calibration in progress .</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Aircraft processor overheated</t>
+          <t>Forward vision sensor calibration error</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>0-4</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1491,17 +1491,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Aircraft processor overheated Automatically returning to home .</t>
+          <t>Forward vision sensor calibration error Auto calibration in progress .</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Automatically returning to home</t>
+          <t>Auto calibration in progress</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3-6</t>
+          <t>5-8</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1516,17 +1516,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Aircraft processor overheated Automatically returning to home .</t>
+          <t>Forward vision sensor calibration error Auto calibration in progress .</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Aircraft processor overheated Automatically returning to home</t>
+          <t>Forward vision sensor calibration error Auto calibration in progress</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0-6</t>
+          <t>0-8</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1541,17 +1541,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Compass Error Compass Redundancy Switch .</t>
+          <t>Critically Low Voltage Aircraft will land .</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Compass Error</t>
+          <t>Critically Low Voltage</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1566,17 +1566,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Compass Error Compass Redundancy Switch .</t>
+          <t>Critically Low Voltage Aircraft will land .</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Compass Redundancy Switch</t>
+          <t>Aircraft will land</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2-4</t>
+          <t>3-5</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1591,17 +1591,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Compass Error Compass Redundancy Switch .</t>
+          <t>Critically Low Voltage Aircraft will land .</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Compass Error Compass Redundancy Switch</t>
+          <t>Critically Low Voltage Aircraft will land</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0-4</t>
+          <t>0-5</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1616,17 +1616,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SD card full Change card or delete files .</t>
+          <t>Attitude is too large Backward Obstacle Sensing is not functioning .</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>SD card full</t>
+          <t>Attitude is too large</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>0-3</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1641,17 +1641,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SD card full Change card or delete files .</t>
+          <t>Attitude is too large Backward Obstacle Sensing is not functioning .</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Change card or delete files</t>
+          <t>Backward Obstacle Sensing is not functioning</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>3-7</t>
+          <t>4-9</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1666,17 +1666,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SD card full Change card or delete files .</t>
+          <t>Attitude is too large Backward Obstacle Sensing is not functioning .</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>SD card full Change card or delete files</t>
+          <t>Attitude is too large Backward Obstacle Sensing is not functioning</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0-7</t>
+          <t>0-9</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1691,12 +1691,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Precision Landing Rectifying aircraft position .</t>
+          <t>Compass Error Compass Redundancy Switch .</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Precision Landing</t>
+          <t>Compass Error</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1716,12 +1716,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Precision Landing Rectifying aircraft position .</t>
+          <t>Compass Error Compass Redundancy Switch .</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Rectifying aircraft position</t>
+          <t>Compass Redundancy Switch</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1741,12 +1741,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Precision Landing Rectifying aircraft position .</t>
+          <t>Compass Error Compass Redundancy Switch .</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Precision Landing Rectifying aircraft position</t>
+          <t>Compass Error Compass Redundancy Switch</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1766,17 +1766,17 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Attitude is too large Backward Obstacle Sensing is not functioning .</t>
+          <t>Aircraft too Far Cannot enter Follow Me Mode .</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Attitude is too large</t>
+          <t>Aircraft too Far</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0-3</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1791,17 +1791,17 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Attitude is too large Backward Obstacle Sensing is not functioning .</t>
+          <t>Aircraft too Far Cannot enter Follow Me Mode .</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Backward Obstacle Sensing is not functioning</t>
+          <t>Cannot enter Follow Me Mode</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>4-9</t>
+          <t>3-7</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1816,17 +1816,17 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Attitude is too large Backward Obstacle Sensing is not functioning .</t>
+          <t>Aircraft too Far Cannot enter Follow Me Mode .</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Attitude is too large Backward Obstacle Sensing is not functioning</t>
+          <t>Aircraft too Far Cannot enter Follow Me Mode</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0-9</t>
+          <t>0-7</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1841,17 +1841,17 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Aircraft too Far Cannot enter Follow Me Mode .</t>
+          <t>Compass Error Compass direction is not the same with IMU .</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Aircraft too Far</t>
+          <t>Compass Error</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1866,17 +1866,17 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Aircraft too Far Cannot enter Follow Me Mode .</t>
+          <t>Compass Error Compass direction is not the same with IMU .</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Cannot enter Follow Me Mode</t>
+          <t>Compass direction is not the same with IMU</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>3-7</t>
+          <t>2-9</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -1891,17 +1891,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Aircraft too Far Cannot enter Follow Me Mode .</t>
+          <t>Compass Error Compass direction is not the same with IMU .</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Aircraft too Far Cannot enter Follow Me Mode</t>
+          <t>Compass Error Compass direction is not the same with IMU</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0-7</t>
+          <t>0-9</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -1916,12 +1916,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Critically low power Aircraft is landing .</t>
+          <t>Aircraft processor overheated Automatically returning to home .</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Critically low power</t>
+          <t>Aircraft processor overheated</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1941,17 +1941,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Critically low power Aircraft is landing .</t>
+          <t>Aircraft processor overheated Automatically returning to home .</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Aircraft is landing</t>
+          <t>Automatically returning to home</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>3-5</t>
+          <t>3-6</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -1966,17 +1966,17 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Critically low power Aircraft is landing .</t>
+          <t>Aircraft processor overheated Automatically returning to home .</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Critically low power Aircraft is landing</t>
+          <t>Aircraft processor overheated Automatically returning to home</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0-5</t>
+          <t>0-6</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -1991,17 +1991,17 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Battery error Aircraft returning to home automatically .</t>
+          <t>Propeller Guard Mounted Propeller Guard mounted Forward Obstacle Sensing will be automatically switched off .</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Battery error</t>
+          <t>Propeller Guard Mounted Propeller Guard mounted</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>0-5</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2016,17 +2016,17 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Battery error Aircraft returning to home automatically .</t>
+          <t>Propeller Guard Mounted Propeller Guard mounted Forward Obstacle Sensing will be automatically switched off .</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Aircraft returning to home automatically</t>
+          <t>Forward Obstacle Sensing will be automatically switched off</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2-6</t>
+          <t>6-13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2041,17 +2041,17 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Battery error Aircraft returning to home automatically .</t>
+          <t>Propeller Guard Mounted Propeller Guard mounted Forward Obstacle Sensing will be automatically switched off .</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Battery error Aircraft returning to home automatically</t>
+          <t>Propeller Guard Mounted Propeller Guard mounted Forward Obstacle Sensing will be automatically switched off</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>0-6</t>
+          <t>0-13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2066,17 +2066,17 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Precision Landing Locating Landing Point .</t>
+          <t>Landing Protection Activated Aircraft will decelerate during landing .</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Precision Landing</t>
+          <t>Landing Protection Activated</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2091,17 +2091,17 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Precision Landing Locating Landing Point .</t>
+          <t>Landing Protection Activated Aircraft will decelerate during landing .</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Locating Landing Point</t>
+          <t>Aircraft will decelerate during landing</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2-4</t>
+          <t>3-7</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2116,17 +2116,17 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Precision Landing Locating Landing Point .</t>
+          <t>Landing Protection Activated Aircraft will decelerate during landing .</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Precision Landing Locating Landing Point</t>
+          <t>Landing Protection Activated Aircraft will decelerate during landing</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>0-4</t>
+          <t>0-7</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">

</xml_diff>